<commit_message>
Adição do texto de conclusão inicial para a comparação entre RVND e ILS
</commit_message>
<xml_diff>
--- a/Arquivos/Análises/Comparação entre RVND e os resultados do artigo.xlsx
+++ b/Arquivos/Análises/Comparação entre RVND e os resultados do artigo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="4785"/>
+    <workbookView windowWidth="13725" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
     <t>ulysses22</t>
   </si>
   <si>
-    <t>Contagem de casos</t>
+    <t>Comparação com os artigos com a RVND</t>
   </si>
   <si>
     <t>Piores</t>
@@ -201,11 +201,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="0_ "/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="24">
@@ -243,9 +243,107 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,15 +366,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -291,97 +381,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -397,96 +397,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,7 +420,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,7 +474,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,7 +498,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +552,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,25 +570,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -724,17 +724,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -758,6 +752,36 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -768,15 +792,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -795,168 +810,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1384,8 +1384,8 @@
   <sheetPr/>
   <dimension ref="B2:X65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P19" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>

</xml_diff>